<commit_message>
updated to handle ways the published value might vary
</commit_message>
<xml_diff>
--- a/spec/fixtures/customers_test.xlsx
+++ b/spec/fixtures/customers_test.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>URN</t>
   </si>
@@ -37,6 +37,9 @@
     <t>Central Government</t>
   </si>
   <si>
+    <t xml:space="preserve">True </t>
+  </si>
+  <si>
     <t>National Museums and Galleries of Wales</t>
   </si>
   <si>
@@ -44,6 +47,15 @@
   </si>
   <si>
     <t>Wider Public Sector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">False </t>
+  </si>
+  <si>
+    <t>Testy McTestface</t>
+  </si>
+  <si>
+    <t>TN34 1RL</t>
   </si>
 </sst>
 </file>
@@ -85,7 +97,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -94,13 +106,19 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -348,8 +366,8 @@
       <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="3" t="b">
-        <v>1</v>
+      <c r="E2" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3">
@@ -357,16 +375,30 @@
         <v>1.0009438E7</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="3" t="b">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6">
+        <v>1.0009439E7</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>